<commit_message>
feat(translation): add translations for 12 languages
</commit_message>
<xml_diff>
--- a/utils/localisation_script/excel_to_json/gu/k.xlsx
+++ b/utils/localisation_script/excel_to_json/gu/k.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/gu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31742B55-ED85-7A45-BB97-9CDF8194AEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7DB543-B6E3-BA48-8943-07AE15DCE680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Page Name</t>
   </si>
   <si>
-    <t>English Copy</t>
-  </si>
-  <si>
     <t>All functional Pages</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>Gujarati</t>
+  </si>
+  <si>
+    <t>English copy</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
   </sheetPr>
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
@@ -579,65 +579,65 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28">
       <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14">
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14">
       <c r="D6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="98">
       <c r="D7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -647,10 +647,10 @@
     </row>
     <row r="9" spans="1:7" ht="14">
       <c r="A9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="10"/>
@@ -679,7 +679,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="12">
         <v>1</v>
@@ -692,14 +692,14 @@
     <row r="13" spans="1:7" ht="98">
       <c r="C13" s="6"/>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14">
@@ -712,7 +712,7 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14">
@@ -720,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="14">
         <v>2</v>
@@ -733,14 +733,14 @@
     <row r="16" spans="1:7" ht="98">
       <c r="C16" s="6"/>
       <c r="D16" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="3:7" ht="14">
@@ -753,7 +753,7 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="3:7" ht="14">
@@ -761,7 +761,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="12">
         <v>3</v>
@@ -774,14 +774,14 @@
     <row r="19" spans="3:7" ht="84">
       <c r="C19" s="6"/>
       <c r="D19" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="14">
@@ -794,7 +794,7 @@
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="3:7" ht="14">
@@ -802,7 +802,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="12">
         <v>4</v>
@@ -815,14 +815,14 @@
     <row r="22" spans="3:7" ht="112">
       <c r="C22" s="6"/>
       <c r="D22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="3:7" ht="14">
@@ -835,7 +835,7 @@
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>